<commit_message>
Refactored helper scripts; started data vis.; continuing report
</commit_message>
<xml_diff>
--- a/data_analysis/elasticity_results/elasticity.xlsx
+++ b/data_analysis/elasticity_results/elasticity.xlsx
@@ -22,319 +22,319 @@
     <t>LatestCensusPop</t>
   </si>
   <si>
-    <t>EstimElasticity</t>
+    <t>Elasticity</t>
+  </si>
+  <si>
+    <t>New Maryland</t>
+  </si>
+  <si>
+    <t>Dorchester</t>
+  </si>
+  <si>
+    <t>Hillsborough</t>
+  </si>
+  <si>
+    <t>Chipman</t>
+  </si>
+  <si>
+    <t>Sackville</t>
+  </si>
+  <si>
+    <t>Maisonnette</t>
+  </si>
+  <si>
+    <t>Paquetville</t>
+  </si>
+  <si>
+    <t>Belledune</t>
+  </si>
+  <si>
+    <t>Blacks Harbour</t>
+  </si>
+  <si>
+    <t>Shippagan</t>
+  </si>
+  <si>
+    <t>Richibucto</t>
+  </si>
+  <si>
+    <t>Clair</t>
+  </si>
+  <si>
+    <t>Sussex Corner</t>
+  </si>
+  <si>
+    <t>Baker-Brook</t>
+  </si>
+  <si>
+    <t>Gagetown</t>
+  </si>
+  <si>
+    <t>Petit-Rocher</t>
+  </si>
+  <si>
+    <t>Kedgwick</t>
+  </si>
+  <si>
+    <t>Oromocto</t>
+  </si>
+  <si>
+    <t>Bertrand</t>
+  </si>
+  <si>
+    <t>Hartland</t>
+  </si>
+  <si>
+    <t>Saint-Léonard</t>
+  </si>
+  <si>
+    <t>Riverside-Albert</t>
+  </si>
+  <si>
+    <t>Millville</t>
+  </si>
+  <si>
+    <t>Shediac</t>
+  </si>
+  <si>
+    <t>Dieppe</t>
+  </si>
+  <si>
+    <t>Quispamsis</t>
+  </si>
+  <si>
+    <t>Caraquet</t>
+  </si>
+  <si>
+    <t>Woodstock</t>
+  </si>
+  <si>
+    <t>Cap-Pelé</t>
+  </si>
+  <si>
+    <t>McAdam</t>
+  </si>
+  <si>
+    <t>Cambridge-Narrows</t>
+  </si>
+  <si>
+    <t>Eel River Crossing</t>
+  </si>
+  <si>
+    <t>Grand Falls/Grand-Sault</t>
+  </si>
+  <si>
+    <t>Plaster Rock</t>
+  </si>
+  <si>
+    <t>Moncton</t>
+  </si>
+  <si>
+    <t>St. Martins</t>
+  </si>
+  <si>
+    <t>Port Elgin</t>
+  </si>
+  <si>
+    <t>Blackville</t>
+  </si>
+  <si>
+    <t>Beresford</t>
+  </si>
+  <si>
+    <t>Aroostook</t>
+  </si>
+  <si>
+    <t>Saint-Hilaire</t>
+  </si>
+  <si>
+    <t>Hampton</t>
+  </si>
+  <si>
+    <t>Saint-François-de-Madawaska</t>
+  </si>
+  <si>
+    <t>Miramichi</t>
+  </si>
+  <si>
+    <t>Salisbury</t>
+  </si>
+  <si>
+    <t>Saint George</t>
+  </si>
+  <si>
+    <t>Saint-Isidore</t>
+  </si>
+  <si>
+    <t>Edmundston</t>
+  </si>
+  <si>
+    <t>Perth-Andover</t>
+  </si>
+  <si>
+    <t>Pointe-Verte</t>
+  </si>
+  <si>
+    <t>Lac Baker</t>
+  </si>
+  <si>
+    <t>Bristol</t>
+  </si>
+  <si>
+    <t>Saint-Louis-de-Kent</t>
+  </si>
+  <si>
+    <t>Saint Andrews</t>
+  </si>
+  <si>
+    <t>Minto</t>
+  </si>
+  <si>
+    <t>Riverview</t>
+  </si>
+  <si>
+    <t>Petitcodiac</t>
+  </si>
+  <si>
+    <t>Canterbury</t>
+  </si>
+  <si>
+    <t>Atholville</t>
+  </si>
+  <si>
+    <t>Rothesay</t>
+  </si>
+  <si>
+    <t>Saint-Quentin</t>
+  </si>
+  <si>
+    <t>Sainte-Marie-Saint-Raphaël</t>
+  </si>
+  <si>
+    <t>Florenceville</t>
+  </si>
+  <si>
+    <t>Harvey</t>
+  </si>
+  <si>
+    <t>Centreville</t>
+  </si>
+  <si>
+    <t>Fredericton Junction</t>
+  </si>
+  <si>
+    <t>Tracadie-Sheila</t>
+  </si>
+  <si>
+    <t>Doaktown</t>
+  </si>
+  <si>
+    <t>Sainte-Anne-de-Madawaska</t>
+  </si>
+  <si>
+    <t>Grande-Anse</t>
+  </si>
+  <si>
+    <t>Rivière-Verte</t>
+  </si>
+  <si>
+    <t>Nackawic</t>
+  </si>
+  <si>
+    <t>Charlo</t>
+  </si>
+  <si>
+    <t>Rogersville</t>
+  </si>
+  <si>
+    <t>Drummond</t>
+  </si>
+  <si>
+    <t>Le Goulet</t>
+  </si>
+  <si>
+    <t>Saint-André</t>
+  </si>
+  <si>
+    <t>Campbellton</t>
+  </si>
+  <si>
+    <t>Bath</t>
+  </si>
+  <si>
+    <t>Grand Manan</t>
+  </si>
+  <si>
+    <t>Alma</t>
+  </si>
+  <si>
+    <t>Rexton</t>
+  </si>
+  <si>
+    <t>Grand Bay-Westfield</t>
+  </si>
+  <si>
+    <t>Norton</t>
+  </si>
+  <si>
+    <t>Bouctouche</t>
+  </si>
+  <si>
+    <t>Bathurst</t>
   </si>
   <si>
     <t>Nigadoo</t>
   </si>
   <si>
-    <t>Minto</t>
-  </si>
-  <si>
-    <t>Riverside-Albert</t>
+    <t>St. Stephen</t>
+  </si>
+  <si>
+    <t>Lamèque</t>
+  </si>
+  <si>
+    <t>Saint John</t>
+  </si>
+  <si>
+    <t>Tracy</t>
+  </si>
+  <si>
+    <t>Florenceville-Bristol</t>
+  </si>
+  <si>
+    <t>Saint-Antoine</t>
+  </si>
+  <si>
+    <t>Memramcook</t>
+  </si>
+  <si>
+    <t>Bas-Caraquet</t>
+  </si>
+  <si>
+    <t>Saint-Léolin</t>
+  </si>
+  <si>
+    <t>Stanley</t>
+  </si>
+  <si>
+    <t>Tide Head</t>
+  </si>
+  <si>
+    <t>Fredericton</t>
   </si>
   <si>
     <t>Dalhousie</t>
   </si>
   <si>
-    <t>Saint-Léonard</t>
-  </si>
-  <si>
-    <t>Alma</t>
-  </si>
-  <si>
-    <t>Eel River Crossing</t>
-  </si>
-  <si>
-    <t>Salisbury</t>
-  </si>
-  <si>
-    <t>Saint-Hilaire</t>
+    <t>Sussex</t>
+  </si>
+  <si>
+    <t>Balmoral</t>
+  </si>
+  <si>
+    <t>Meductic</t>
   </si>
   <si>
     <t>Néguac</t>
-  </si>
-  <si>
-    <t>Florenceville</t>
-  </si>
-  <si>
-    <t>Drummond</t>
-  </si>
-  <si>
-    <t>Perth-Andover</t>
-  </si>
-  <si>
-    <t>Port Elgin</t>
-  </si>
-  <si>
-    <t>Bas-Caraquet</t>
-  </si>
-  <si>
-    <t>Shediac</t>
-  </si>
-  <si>
-    <t>Hampton</t>
-  </si>
-  <si>
-    <t>Saint-Antoine</t>
-  </si>
-  <si>
-    <t>St. Martins</t>
-  </si>
-  <si>
-    <t>Sussex</t>
-  </si>
-  <si>
-    <t>Quispamsis</t>
-  </si>
-  <si>
-    <t>McAdam</t>
-  </si>
-  <si>
-    <t>Fredericton</t>
-  </si>
-  <si>
-    <t>Saint George</t>
-  </si>
-  <si>
-    <t>Saint-Léolin</t>
-  </si>
-  <si>
-    <t>Sussex Corner</t>
-  </si>
-  <si>
-    <t>Bathurst</t>
-  </si>
-  <si>
-    <t>Memramcook</t>
-  </si>
-  <si>
-    <t>Harvey</t>
-  </si>
-  <si>
-    <t>Plaster Rock</t>
-  </si>
-  <si>
-    <t>Gagetown</t>
-  </si>
-  <si>
-    <t>Millville</t>
-  </si>
-  <si>
-    <t>Rexton</t>
-  </si>
-  <si>
-    <t>Fredericton Junction</t>
-  </si>
-  <si>
-    <t>Petitcodiac</t>
-  </si>
-  <si>
-    <t>Paquetville</t>
-  </si>
-  <si>
-    <t>St. Stephen</t>
-  </si>
-  <si>
-    <t>Beresford</t>
-  </si>
-  <si>
-    <t>Saint John</t>
-  </si>
-  <si>
-    <t>Bristol</t>
-  </si>
-  <si>
-    <t>Sainte-Anne-de-Madawaska</t>
-  </si>
-  <si>
-    <t>Norton</t>
-  </si>
-  <si>
-    <t>Cap-Pelé</t>
-  </si>
-  <si>
-    <t>Hartland</t>
-  </si>
-  <si>
-    <t>Lac Baker</t>
-  </si>
-  <si>
-    <t>Nackawic</t>
-  </si>
-  <si>
-    <t>Saint Andrews</t>
-  </si>
-  <si>
-    <t>Chipman</t>
-  </si>
-  <si>
-    <t>Bertrand</t>
-  </si>
-  <si>
-    <t>Richibucto</t>
-  </si>
-  <si>
-    <t>Sainte-Marie-Saint-Raphaël</t>
-  </si>
-  <si>
-    <t>Saint-Quentin</t>
-  </si>
-  <si>
-    <t>Sackville</t>
-  </si>
-  <si>
-    <t>Le Goulet</t>
-  </si>
-  <si>
-    <t>Clair</t>
-  </si>
-  <si>
-    <t>Florenceville-Bristol</t>
-  </si>
-  <si>
-    <t>Doaktown</t>
-  </si>
-  <si>
-    <t>Charlo</t>
-  </si>
-  <si>
-    <t>Baker-Brook</t>
-  </si>
-  <si>
-    <t>Shippagan</t>
-  </si>
-  <si>
-    <t>Bath</t>
-  </si>
-  <si>
-    <t>Rogersville</t>
-  </si>
-  <si>
-    <t>Tracy</t>
-  </si>
-  <si>
-    <t>Tracadie-Sheila</t>
-  </si>
-  <si>
-    <t>Hillsborough</t>
-  </si>
-  <si>
-    <t>Saint-André</t>
-  </si>
-  <si>
-    <t>New Maryland</t>
-  </si>
-  <si>
-    <t>Kedgwick</t>
-  </si>
-  <si>
-    <t>Riverview</t>
-  </si>
-  <si>
-    <t>Canterbury</t>
-  </si>
-  <si>
-    <t>Grand Manan</t>
-  </si>
-  <si>
-    <t>Moncton</t>
-  </si>
-  <si>
-    <t>Blacks Harbour</t>
-  </si>
-  <si>
-    <t>Centreville</t>
-  </si>
-  <si>
-    <t>Tide Head</t>
-  </si>
-  <si>
-    <t>Lamèque</t>
-  </si>
-  <si>
-    <t>Grande-Anse</t>
-  </si>
-  <si>
-    <t>Miramichi</t>
-  </si>
-  <si>
-    <t>Aroostook</t>
-  </si>
-  <si>
-    <t>Stanley</t>
-  </si>
-  <si>
-    <t>Rivière-Verte</t>
-  </si>
-  <si>
-    <t>Grand Falls/Grand-Sault</t>
-  </si>
-  <si>
-    <t>Saint-Louis-de-Kent</t>
-  </si>
-  <si>
-    <t>Balmoral</t>
-  </si>
-  <si>
-    <t>Cambridge-Narrows</t>
-  </si>
-  <si>
-    <t>Campbellton</t>
-  </si>
-  <si>
-    <t>Dorchester</t>
-  </si>
-  <si>
-    <t>Edmundston</t>
-  </si>
-  <si>
-    <t>Meductic</t>
-  </si>
-  <si>
-    <t>Dieppe</t>
-  </si>
-  <si>
-    <t>Bouctouche</t>
-  </si>
-  <si>
-    <t>Pointe-Verte</t>
-  </si>
-  <si>
-    <t>Blackville</t>
-  </si>
-  <si>
-    <t>Caraquet</t>
-  </si>
-  <si>
-    <t>Atholville</t>
-  </si>
-  <si>
-    <t>Saint-François-de-Madawaska</t>
-  </si>
-  <si>
-    <t>Oromocto</t>
-  </si>
-  <si>
-    <t>Woodstock</t>
-  </si>
-  <si>
-    <t>Petit-Rocher</t>
-  </si>
-  <si>
-    <t>Rothesay</t>
-  </si>
-  <si>
-    <t>Saint-Isidore</t>
-  </si>
-  <si>
-    <t>Maisonnette</t>
-  </si>
-  <si>
-    <t>Belledune</t>
-  </si>
-  <si>
-    <t>Grand Bay-Westfield</t>
   </si>
 </sst>
 </file>
@@ -410,7 +410,7 @@
   <tableColumns count="3">
     <tableColumn id="1" name="Municipality" dataDxfId="0"/>
     <tableColumn id="2" name="LatestCensusPop" dataDxfId="1"/>
-    <tableColumn id="3" name="EstimElasticity" dataDxfId="1"/>
+    <tableColumn id="3" name="Elasticity" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -709,7 +709,7 @@
   <cols>
     <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -728,10 +728,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="3">
-        <v>953.5555555555555</v>
+        <v>4244.111111111111</v>
       </c>
       <c r="C2" s="3">
-        <v>4.038310731320847</v>
+        <v>1.952990849728095</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -739,10 +739,10 @@
         <v>4</v>
       </c>
       <c r="B3" s="3">
-        <v>2657.555555555556</v>
+        <v>1108.333333333333</v>
       </c>
       <c r="C3" s="3">
-        <v>4.197586631988713</v>
+        <v>4.37942380018478</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -750,10 +750,10 @@
         <v>5</v>
       </c>
       <c r="B4" s="3">
-        <v>360.3333333333333</v>
+        <v>1298.388888888889</v>
       </c>
       <c r="C4" s="3">
-        <v>3.257283448665551</v>
+        <v>3.176899455564953</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -761,10 +761,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="3">
-        <v>3735.055555555556</v>
+        <v>1308.944444444444</v>
       </c>
       <c r="C5" s="3">
-        <v>1.624471405454341</v>
+        <v>2.978555887229455</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -772,10 +772,10 @@
         <v>7</v>
       </c>
       <c r="B6" s="3">
-        <v>1363.166666666667</v>
+        <v>5419</v>
       </c>
       <c r="C6" s="3">
-        <v>3.418843430950351</v>
+        <v>1.173257410267234</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -783,10 +783,10 @@
         <v>8</v>
       </c>
       <c r="B7" s="3">
-        <v>271</v>
+        <v>589.5555555555555</v>
       </c>
       <c r="C7" s="3">
-        <v>1.357267809395548</v>
+        <v>4.246522363577463</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -794,10 +794,10 @@
         <v>9</v>
       </c>
       <c r="B8" s="3">
-        <v>1382.111111111111</v>
+        <v>688.2222222222222</v>
       </c>
       <c r="C8" s="3">
-        <v>4.898511730109933</v>
+        <v>2.704154469791415</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -805,10 +805,10 @@
         <v>10</v>
       </c>
       <c r="B9" s="3">
-        <v>2075.555555555556</v>
+        <v>1719.277777777778</v>
       </c>
       <c r="C9" s="3">
-        <v>2.260287591483114</v>
+        <v>-0.03230382618528604</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -816,10 +816,10 @@
         <v>11</v>
       </c>
       <c r="B10" s="3">
-        <v>246.4117647058823</v>
+        <v>1003.333333333333</v>
       </c>
       <c r="C10" s="3">
-        <v>1.158134751276184</v>
+        <v>2.327125813468714</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -827,10 +827,10 @@
         <v>12</v>
       </c>
       <c r="B11" s="3">
-        <v>1676.388888888889</v>
+        <v>2741.777777777778</v>
       </c>
       <c r="C11" s="3">
-        <v>2.591587053447861</v>
+        <v>1.826592004438217</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -838,10 +838,10 @@
         <v>13</v>
       </c>
       <c r="B12" s="3">
-        <v>765.875</v>
+        <v>1314.277777777778</v>
       </c>
       <c r="C12" s="3">
-        <v>0.573127290007251</v>
+        <v>1.865748618876328</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -849,10 +849,10 @@
         <v>14</v>
       </c>
       <c r="B13" s="3">
-        <v>847.2777777777778</v>
+        <v>854.9411764705883</v>
       </c>
       <c r="C13" s="3">
-        <v>2.572049085509784</v>
+        <v>2.194402962374678</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -860,10 +860,10 @@
         <v>15</v>
       </c>
       <c r="B14" s="3">
-        <v>1787.444444444444</v>
+        <v>1411.222222222222</v>
       </c>
       <c r="C14" s="3">
-        <v>2.554189517200615</v>
+        <v>2.741347663741911</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -871,10 +871,10 @@
         <v>16</v>
       </c>
       <c r="B15" s="3">
-        <v>433</v>
+        <v>575.1176470588235</v>
       </c>
       <c r="C15" s="3">
-        <v>3.283557924396782</v>
+        <v>3.945005804783354</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -882,10 +882,10 @@
         <v>17</v>
       </c>
       <c r="B16" s="3">
-        <v>1510.111111111111</v>
+        <v>697</v>
       </c>
       <c r="C16" s="3">
-        <v>4.546177680392857</v>
+        <v>1.94581028903611</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -893,10 +893,10 @@
         <v>18</v>
       </c>
       <c r="B17" s="3">
-        <v>5576.888888888889</v>
+        <v>1955.555555555556</v>
       </c>
       <c r="C17" s="3">
-        <v>1.586339013573295</v>
+        <v>3.707019874209061</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -904,10 +904,10 @@
         <v>19</v>
       </c>
       <c r="B18" s="3">
-        <v>4127.166666666667</v>
+        <v>1161.5</v>
       </c>
       <c r="C18" s="3">
-        <v>2.115598367972202</v>
+        <v>4.910995710330457</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -915,10 +915,10 @@
         <v>20</v>
       </c>
       <c r="B19" s="3">
-        <v>1599.111111111111</v>
+        <v>8862.111111111111</v>
       </c>
       <c r="C19" s="3">
-        <v>2.981165133876113</v>
+        <v>1.015540391140557</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -926,10 +926,10 @@
         <v>21</v>
       </c>
       <c r="B20" s="3">
-        <v>349.6666666666667</v>
+        <v>1215.833333333333</v>
       </c>
       <c r="C20" s="3">
-        <v>2.678958345188971</v>
+        <v>4.520087914571928</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -937,10 +937,10 @@
         <v>22</v>
       </c>
       <c r="B21" s="3">
-        <v>4262.444444444444</v>
+        <v>932</v>
       </c>
       <c r="C21" s="3">
-        <v>1.518741451488723</v>
+        <v>1.756911632289728</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -948,10 +948,10 @@
         <v>23</v>
       </c>
       <c r="B22" s="3">
-        <v>15794.88888888889</v>
+        <v>1363.166666666667</v>
       </c>
       <c r="C22" s="3">
-        <v>1.732099193608482</v>
+        <v>3.418821882174067</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -959,10 +959,10 @@
         <v>24</v>
       </c>
       <c r="B23" s="3">
-        <v>1381</v>
+        <v>360.3333333333333</v>
       </c>
       <c r="C23" s="3">
-        <v>5.41828501472102</v>
+        <v>3.257262687746987</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -970,10 +970,10 @@
         <v>25</v>
       </c>
       <c r="B24" s="3">
-        <v>52043.83333333334</v>
+        <v>304.5555555555555</v>
       </c>
       <c r="C24" s="3">
-        <v>0.9589738640101915</v>
+        <v>5.423905213307876</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -981,10 +981,10 @@
         <v>26</v>
       </c>
       <c r="B25" s="3">
-        <v>1480.333333333333</v>
+        <v>5576.888888888889</v>
       </c>
       <c r="C25" s="3">
-        <v>1.692940641518225</v>
+        <v>1.586326401123529</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -992,10 +992,10 @@
         <v>27</v>
       </c>
       <c r="B26" s="3">
-        <v>718.3333333333334</v>
+        <v>19142.27777777778</v>
       </c>
       <c r="C26" s="3">
-        <v>7.020142846174499</v>
+        <v>0.9990234685779513</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1003,10 +1003,10 @@
         <v>28</v>
       </c>
       <c r="B27" s="3">
-        <v>1411.222222222222</v>
+        <v>15794.88888888889</v>
       </c>
       <c r="C27" s="3">
-        <v>2.741365908755164</v>
+        <v>1.732085870349754</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1014,10 +1014,10 @@
         <v>29</v>
       </c>
       <c r="B28" s="3">
-        <v>12698.77777777778</v>
+        <v>4304.722222222223</v>
       </c>
       <c r="C28" s="3">
-        <v>1.783880159432867</v>
+        <v>2.060478459612275</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -1025,10 +1025,10 @@
         <v>30</v>
       </c>
       <c r="B29" s="3">
-        <v>4762.055555555556</v>
+        <v>5174.166666666667</v>
       </c>
       <c r="C29" s="3">
-        <v>3.281256430878462</v>
+        <v>1.701667528830308</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1036,10 +1036,10 @@
         <v>31</v>
       </c>
       <c r="B30" s="3">
-        <v>360.1111111111111</v>
+        <v>2289.888888888889</v>
       </c>
       <c r="C30" s="3">
-        <v>3.39135325692596</v>
+        <v>2.114770802958085</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1047,10 +1047,10 @@
         <v>32</v>
       </c>
       <c r="B31" s="3">
-        <v>1148.666666666667</v>
+        <v>1381</v>
       </c>
       <c r="C31" s="3">
-        <v>2.967219084668789</v>
+        <v>5.41825371553831</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1058,10 +1058,10 @@
         <v>33</v>
       </c>
       <c r="B32" s="3">
-        <v>697</v>
+        <v>645.2777777777778</v>
       </c>
       <c r="C32" s="3">
-        <v>1.945824654540896</v>
+        <v>0.8796179759578735</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1069,10 +1069,10 @@
         <v>34</v>
       </c>
       <c r="B33" s="3">
-        <v>304.5555555555555</v>
+        <v>1382.111111111111</v>
       </c>
       <c r="C33" s="3">
-        <v>5.423936540050615</v>
+        <v>4.898482965635322</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1080,10 +1080,10 @@
         <v>35</v>
       </c>
       <c r="B34" s="3">
-        <v>845.8888888888889</v>
+        <v>5723.611111111111</v>
       </c>
       <c r="C34" s="3">
-        <v>1.809903866792523</v>
+        <v>1.509234673336074</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1091,10 +1091,10 @@
         <v>36</v>
       </c>
       <c r="B35" s="3">
-        <v>721.0555555555555</v>
+        <v>1148.666666666667</v>
       </c>
       <c r="C35" s="3">
-        <v>3.327960062083229</v>
+        <v>2.96719973826789</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1102,10 +1102,10 @@
         <v>37</v>
       </c>
       <c r="B36" s="3">
-        <v>1406.222222222222</v>
+        <v>65204.44444444445</v>
       </c>
       <c r="C36" s="3">
-        <v>2.606748972727698</v>
+        <v>1.277468593367812</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1113,10 +1113,10 @@
         <v>38</v>
       </c>
       <c r="B37" s="3">
-        <v>688.2222222222222</v>
+        <v>349.6666666666667</v>
       </c>
       <c r="C37" s="3">
-        <v>2.704172533428764</v>
+        <v>2.678940404510244</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1124,10 +1124,10 @@
         <v>39</v>
       </c>
       <c r="B38" s="3">
-        <v>4738.722222222223</v>
+        <v>433</v>
       </c>
       <c r="C38" s="3">
-        <v>2.020912869156378</v>
+        <v>3.283537035349036</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1135,10 +1135,10 @@
         <v>40</v>
       </c>
       <c r="B39" s="3">
-        <v>4388.333333333333</v>
+        <v>966.9444444444445</v>
       </c>
       <c r="C39" s="3">
-        <v>3.15458646616991</v>
+        <v>3.633383811351338</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1146,10 +1146,10 @@
         <v>41</v>
       </c>
       <c r="B40" s="3">
-        <v>69425.38888888889</v>
+        <v>4388.333333333333</v>
       </c>
       <c r="C40" s="3">
-        <v>1.47348818993047</v>
+        <v>3.154566206059836</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1157,10 +1157,10 @@
         <v>42</v>
       </c>
       <c r="B41" s="3">
-        <v>704.5</v>
+        <v>354.6111111111111</v>
       </c>
       <c r="C41" s="3">
-        <v>2.838673628032749</v>
+        <v>6.887094143371944</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1168,10 +1168,10 @@
         <v>43</v>
       </c>
       <c r="B42" s="3">
-        <v>1087.055555555556</v>
+        <v>246.4117647058823</v>
       </c>
       <c r="C42" s="3">
-        <v>4.759603374997129</v>
+        <v>1.158124226992246</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1179,10 +1179,10 @@
         <v>44</v>
       </c>
       <c r="B43" s="3">
-        <v>1344.444444444444</v>
+        <v>4127.166666666667</v>
       </c>
       <c r="C43" s="3">
-        <v>3.921850185297906</v>
+        <v>2.115583174554904</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1190,10 +1190,10 @@
         <v>45</v>
       </c>
       <c r="B44" s="3">
-        <v>2289.888888888889</v>
+        <v>565.0588235294117</v>
       </c>
       <c r="C44" s="3">
-        <v>2.114785992413782</v>
+        <v>2.264175256123465</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1201,10 +1201,10 @@
         <v>46</v>
       </c>
       <c r="B45" s="3">
-        <v>932</v>
+        <v>18208.16666666667</v>
       </c>
       <c r="C45" s="3">
-        <v>1.756925076613483</v>
+        <v>1.784736035585024</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1212,10 +1212,10 @@
         <v>47</v>
       </c>
       <c r="B46" s="3">
-        <v>489.0555555555555</v>
+        <v>2075.555555555556</v>
       </c>
       <c r="C46" s="3">
-        <v>3.008857718186561</v>
+        <v>2.260271692479443</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1223,10 +1223,10 @@
         <v>48</v>
       </c>
       <c r="B47" s="3">
-        <v>1029.5</v>
+        <v>1480.333333333333</v>
       </c>
       <c r="C47" s="3">
-        <v>0.9283808435751242</v>
+        <v>1.692927509218713</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1234,10 +1234,10 @@
         <v>49</v>
       </c>
       <c r="B48" s="3">
-        <v>1820.388888888889</v>
+        <v>812.8333333333334</v>
       </c>
       <c r="C48" s="3">
-        <v>0.571318816451015</v>
+        <v>3.336739651606498</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1245,10 +1245,10 @@
         <v>50</v>
       </c>
       <c r="B49" s="3">
-        <v>1308.944444444444</v>
+        <v>16813.55555555555</v>
       </c>
       <c r="C49" s="3">
-        <v>2.97857528900962</v>
+        <v>1.824416770379819</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1256,10 +1256,10 @@
         <v>51</v>
       </c>
       <c r="B50" s="3">
-        <v>1215.833333333333</v>
+        <v>1787.444444444444</v>
       </c>
       <c r="C50" s="3">
-        <v>4.520114833769558</v>
+        <v>2.554172184965163</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1267,10 +1267,10 @@
         <v>52</v>
       </c>
       <c r="B51" s="3">
-        <v>1314.277777777778</v>
+        <v>994.7777777777778</v>
       </c>
       <c r="C51" s="3">
-        <v>1.865762593953287</v>
+        <v>5.274725717453601</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1278,10 +1278,10 @@
         <v>53</v>
       </c>
       <c r="B52" s="3">
-        <v>1021.222222222222</v>
+        <v>489.0555555555555</v>
       </c>
       <c r="C52" s="3">
-        <v>6.007661663351533</v>
+        <v>3.008838168732169</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1289,10 +1289,10 @@
         <v>54</v>
       </c>
       <c r="B53" s="3">
-        <v>2240.222222222222</v>
+        <v>704.5</v>
       </c>
       <c r="C53" s="3">
-        <v>3.087083424359087</v>
+        <v>2.838654908492098</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1300,10 +1300,10 @@
         <v>55</v>
       </c>
       <c r="B54" s="3">
-        <v>5419</v>
+        <v>950.3333333333334</v>
       </c>
       <c r="C54" s="3">
-        <v>1.173268008349481</v>
+        <v>2.968406732834274</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1311,10 +1311,10 @@
         <v>56</v>
       </c>
       <c r="B55" s="3">
-        <v>898.9444444444445</v>
+        <v>1820.388888888889</v>
       </c>
       <c r="C55" s="3">
-        <v>8.023176543323974</v>
+        <v>0.571311153813002</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1322,10 +1322,10 @@
         <v>57</v>
       </c>
       <c r="B56" s="3">
-        <v>854.9411764705883</v>
+        <v>2657.555555555556</v>
       </c>
       <c r="C56" s="3">
-        <v>2.194418540163653</v>
+        <v>4.197561285620755</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1333,10 +1333,10 @@
         <v>58</v>
       </c>
       <c r="B57" s="3">
-        <v>1598.5</v>
+        <v>18092.33333333333</v>
       </c>
       <c r="C57" s="3">
-        <v>0.5343443932034462</v>
+        <v>2.276943870757617</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1344,10 +1344,10 @@
         <v>59</v>
       </c>
       <c r="B58" s="3">
-        <v>878.3888888888889</v>
+        <v>1406.222222222222</v>
       </c>
       <c r="C58" s="3">
-        <v>2.269563077876119</v>
+        <v>2.606731384182654</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1355,10 +1355,10 @@
         <v>60</v>
       </c>
       <c r="B59" s="3">
-        <v>1404.611111111111</v>
+        <v>366.0555555555555</v>
       </c>
       <c r="C59" s="3">
-        <v>3.339460751611919</v>
+        <v>5.145604421258335</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1366,10 +1366,10 @@
         <v>61</v>
       </c>
       <c r="B60" s="3">
-        <v>575.1176470588235</v>
+        <v>1695.222222222222</v>
       </c>
       <c r="C60" s="3">
-        <v>3.94502991954214</v>
+        <v>0.9621589682907417</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1377,10 +1377,10 @@
         <v>62</v>
       </c>
       <c r="B61" s="3">
-        <v>2741.777777777778</v>
+        <v>11635.55555555555</v>
       </c>
       <c r="C61" s="3">
-        <v>1.826605788564478</v>
+        <v>1.409696492634694</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1388,10 +1388,10 @@
         <v>63</v>
       </c>
       <c r="B62" s="3">
-        <v>543.2777777777778</v>
+        <v>2240.222222222222</v>
       </c>
       <c r="C62" s="3">
-        <v>3.8898942454516</v>
+        <v>3.08706349343197</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1399,10 +1399,10 @@
         <v>64</v>
       </c>
       <c r="B63" s="3">
-        <v>1208.611111111111</v>
+        <v>1021.222222222222</v>
       </c>
       <c r="C63" s="3">
-        <v>4.085206647051892</v>
+        <v>6.007627490035411</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1410,10 +1410,10 @@
         <v>65</v>
       </c>
       <c r="B64" s="3">
-        <v>610.0555555555555</v>
+        <v>765.875</v>
       </c>
       <c r="C64" s="3">
-        <v>4.675517318414739</v>
+        <v>0.5731196185501</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1421,10 +1421,10 @@
         <v>66</v>
       </c>
       <c r="B65" s="3">
-        <v>4690</v>
+        <v>360.1111111111111</v>
       </c>
       <c r="C65" s="3">
-        <v>1.939962468432902</v>
+        <v>3.39133184220729</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1432,10 +1432,10 @@
         <v>67</v>
       </c>
       <c r="B66" s="3">
-        <v>1298.388888888889</v>
+        <v>540.8888888888889</v>
       </c>
       <c r="C66" s="3">
-        <v>3.176919824585096</v>
+        <v>2.262430506182488</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1443,10 +1443,10 @@
         <v>68</v>
       </c>
       <c r="B67" s="3">
-        <v>426.5</v>
+        <v>721.0555555555555</v>
       </c>
       <c r="C67" s="3">
-        <v>4.635821038384033</v>
+        <v>3.327938956505582</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1454,10 +1454,10 @@
         <v>69</v>
       </c>
       <c r="B68" s="3">
-        <v>4244.111111111111</v>
+        <v>4690</v>
       </c>
       <c r="C68" s="3">
-        <v>1.95300525024952</v>
+        <v>1.939948131515448</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1465,10 +1465,10 @@
         <v>70</v>
       </c>
       <c r="B69" s="3">
-        <v>1161.5</v>
+        <v>878.3888888888889</v>
       </c>
       <c r="C69" s="3">
-        <v>4.911024535824577</v>
+        <v>2.269547133639938</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1476,10 +1476,10 @@
         <v>71</v>
       </c>
       <c r="B70" s="3">
-        <v>18092.33333333333</v>
+        <v>1087.055555555556</v>
       </c>
       <c r="C70" s="3">
-        <v>2.276959851064642</v>
+        <v>4.759575287918111</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1487,10 +1487,10 @@
         <v>72</v>
       </c>
       <c r="B71" s="3">
-        <v>366.0555555555555</v>
+        <v>827.3888888888889</v>
       </c>
       <c r="C71" s="3">
-        <v>5.145634390842613</v>
+        <v>3.933745317083301</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -1498,10 +1498,10 @@
         <v>73</v>
       </c>
       <c r="B72" s="3">
-        <v>2469.388888888889</v>
+        <v>805.1666666666666</v>
       </c>
       <c r="C72" s="3">
-        <v>2.13155455702909</v>
+        <v>3.882179446133341</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -1509,10 +1509,10 @@
         <v>74</v>
       </c>
       <c r="B73" s="3">
-        <v>65204.44444444445</v>
+        <v>1029.5</v>
       </c>
       <c r="C73" s="3">
-        <v>1.277479699645124</v>
+        <v>0.9283714397010021</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -1520,10 +1520,10 @@
         <v>75</v>
       </c>
       <c r="B74" s="3">
-        <v>1003.333333333333</v>
+        <v>1404.611111111111</v>
       </c>
       <c r="C74" s="3">
-        <v>2.327142038492427</v>
+        <v>3.339439589950414</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -1531,10 +1531,10 @@
         <v>76</v>
       </c>
       <c r="B75" s="3">
-        <v>540.8888888888889</v>
+        <v>1208.611111111111</v>
       </c>
       <c r="C75" s="3">
-        <v>2.262446415713805</v>
+        <v>4.085181848712212</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -1542,10 +1542,10 @@
         <v>77</v>
       </c>
       <c r="B76" s="3">
-        <v>1071.666666666667</v>
+        <v>847.2777777777778</v>
       </c>
       <c r="C76" s="3">
-        <v>3.382899865473342</v>
+        <v>2.572031666180989</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -1553,10 +1553,10 @@
         <v>78</v>
       </c>
       <c r="B77" s="3">
-        <v>1469.222222222222</v>
+        <v>898.9444444444445</v>
       </c>
       <c r="C77" s="3">
-        <v>2.720363299132652</v>
+        <v>8.023132541218956</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -1564,10 +1564,10 @@
         <v>79</v>
       </c>
       <c r="B78" s="3">
-        <v>827.3888888888889</v>
+        <v>426.5</v>
       </c>
       <c r="C78" s="3">
-        <v>3.933769376929322</v>
+        <v>4.635793554937599</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -1575,10 +1575,10 @@
         <v>80</v>
       </c>
       <c r="B79" s="3">
-        <v>18208.16666666667</v>
+        <v>7539.722222222223</v>
       </c>
       <c r="C79" s="3">
-        <v>1.784749615596946</v>
+        <v>2.369143003552924</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -1586,10 +1586,10 @@
         <v>81</v>
       </c>
       <c r="B80" s="3">
-        <v>354.6111111111111</v>
+        <v>543.2777777777778</v>
       </c>
       <c r="C80" s="3">
-        <v>6.887132605485095</v>
+        <v>3.8898703995655</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -1597,10 +1597,10 @@
         <v>82</v>
       </c>
       <c r="B81" s="3">
-        <v>429.7222222222222</v>
+        <v>2469.388888888889</v>
       </c>
       <c r="C81" s="3">
-        <v>2.454649513814003</v>
+        <v>2.131539285800402</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -1608,10 +1608,10 @@
         <v>83</v>
       </c>
       <c r="B82" s="3">
-        <v>805.1666666666666</v>
+        <v>271</v>
       </c>
       <c r="C82" s="3">
-        <v>3.882203254513826</v>
+        <v>1.35725631402635</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -1619,10 +1619,10 @@
         <v>84</v>
       </c>
       <c r="B83" s="3">
-        <v>5723.611111111111</v>
+        <v>845.8888888888889</v>
       </c>
       <c r="C83" s="3">
-        <v>1.509246909841202</v>
+        <v>1.809890164114266</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -1630,10 +1630,10 @@
         <v>85</v>
       </c>
       <c r="B84" s="3">
-        <v>950.3333333333334</v>
+        <v>4986.222222222223</v>
       </c>
       <c r="C84" s="3">
-        <v>2.968426085121189</v>
+        <v>2.416673700971703</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -1641,10 +1641,10 @@
         <v>86</v>
       </c>
       <c r="B85" s="3">
-        <v>1770.055555555556</v>
+        <v>1344.444444444444</v>
       </c>
       <c r="C85" s="3">
-        <v>3.998279421613637</v>
+        <v>3.921826183576595</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -1652,10 +1652,10 @@
         <v>87</v>
       </c>
       <c r="B86" s="3">
-        <v>645.2777777777778</v>
+        <v>2408.055555555556</v>
       </c>
       <c r="C86" s="3">
-        <v>0.879627142081411</v>
+        <v>1.940028840493857</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -1663,10 +1663,10 @@
         <v>88</v>
       </c>
       <c r="B87" s="3">
-        <v>7539.722222222223</v>
+        <v>12698.77777777778</v>
       </c>
       <c r="C87" s="3">
-        <v>2.369159433477187</v>
+        <v>1.783866583660905</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -1674,10 +1674,10 @@
         <v>89</v>
       </c>
       <c r="B88" s="3">
-        <v>1108.333333333333</v>
+        <v>953.5555555555555</v>
       </c>
       <c r="C88" s="3">
-        <v>4.379450033421398</v>
+        <v>4.038286161672137</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -1685,10 +1685,10 @@
         <v>90</v>
       </c>
       <c r="B89" s="3">
-        <v>16813.55555555555</v>
+        <v>4738.722222222223</v>
       </c>
       <c r="C89" s="3">
-        <v>1.824430543898358</v>
+        <v>2.020898137479048</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -1696,10 +1696,10 @@
         <v>91</v>
       </c>
       <c r="B90" s="3">
-        <v>198.0555555555555</v>
+        <v>1469.222222222222</v>
       </c>
       <c r="C90" s="3">
-        <v>2.11475624259134</v>
+        <v>2.720345156539985</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -1707,10 +1707,10 @@
         <v>92</v>
       </c>
       <c r="B91" s="3">
-        <v>19142.27777777778</v>
+        <v>69425.38888888889</v>
       </c>
       <c r="C91" s="3">
-        <v>0.9990332169929497</v>
+        <v>1.473476127805057</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -1718,10 +1718,10 @@
         <v>93</v>
       </c>
       <c r="B92" s="3">
-        <v>2408.055555555556</v>
+        <v>610.0555555555555</v>
       </c>
       <c r="C92" s="3">
-        <v>1.940043177804896</v>
+        <v>4.675489641386824</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -1729,10 +1729,10 @@
         <v>94</v>
       </c>
       <c r="B93" s="3">
-        <v>994.7777777777778</v>
+        <v>1598.5</v>
       </c>
       <c r="C93" s="3">
-        <v>5.274756316709316</v>
+        <v>0.5343369108736038</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -1740,10 +1740,10 @@
         <v>95</v>
       </c>
       <c r="B94" s="3">
-        <v>966.9444444444445</v>
+        <v>1599.111111111111</v>
       </c>
       <c r="C94" s="3">
-        <v>3.633406406457873</v>
+        <v>2.981145719466401</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -1751,10 +1751,10 @@
         <v>96</v>
       </c>
       <c r="B95" s="3">
-        <v>4304.722222222223</v>
+        <v>4762.055555555556</v>
       </c>
       <c r="C95" s="3">
-        <v>2.06049338430655</v>
+        <v>3.281235553054098</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -1762,10 +1762,10 @@
         <v>97</v>
       </c>
       <c r="B96" s="3">
-        <v>1695.222222222222</v>
+        <v>1510.111111111111</v>
       </c>
       <c r="C96" s="3">
-        <v>0.9621685369327393</v>
+        <v>4.546150634098066</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -1773,10 +1773,10 @@
         <v>98</v>
       </c>
       <c r="B97" s="3">
-        <v>565.0588235294117</v>
+        <v>718.3333333333334</v>
       </c>
       <c r="C97" s="3">
-        <v>2.26419117416321</v>
+        <v>7.020103735428291</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -1784,10 +1784,10 @@
         <v>99</v>
       </c>
       <c r="B98" s="3">
-        <v>8862.111111111111</v>
+        <v>429.7222222222222</v>
       </c>
       <c r="C98" s="3">
-        <v>1.015550220101792</v>
+        <v>2.454632666991825</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -1795,10 +1795,10 @@
         <v>100</v>
       </c>
       <c r="B99" s="3">
-        <v>5174.166666666667</v>
+        <v>1071.666666666667</v>
       </c>
       <c r="C99" s="3">
-        <v>1.701680703751299</v>
+        <v>3.382878491978183</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -1806,10 +1806,10 @@
         <v>101</v>
       </c>
       <c r="B100" s="3">
-        <v>1955.555555555556</v>
+        <v>52043.83333333334</v>
       </c>
       <c r="C100" s="3">
-        <v>3.707042828408379</v>
+        <v>0.9589643109472232</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -1817,10 +1817,10 @@
         <v>102</v>
       </c>
       <c r="B101" s="3">
-        <v>11635.55555555555</v>
+        <v>3735.055555555556</v>
       </c>
       <c r="C101" s="3">
-        <v>1.409708243733068</v>
+        <v>1.624458607049494</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -1828,10 +1828,10 @@
         <v>103</v>
       </c>
       <c r="B102" s="3">
-        <v>812.8333333333334</v>
+        <v>4262.444444444444</v>
       </c>
       <c r="C102" s="3">
-        <v>3.336760800101516</v>
+        <v>1.518729168682847</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -1839,10 +1839,10 @@
         <v>104</v>
       </c>
       <c r="B103" s="3">
-        <v>589.5555555555555</v>
+        <v>1770.055555555556</v>
       </c>
       <c r="C103" s="3">
-        <v>4.246547948708454</v>
+        <v>3.998255047180202</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -1850,10 +1850,10 @@
         <v>105</v>
       </c>
       <c r="B104" s="3">
-        <v>1719.277777777778</v>
+        <v>198.0555555555555</v>
       </c>
       <c r="C104" s="3">
-        <v>-0.03229910712918538</v>
+        <v>2.114741053280721</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -1861,10 +1861,10 @@
         <v>106</v>
       </c>
       <c r="B105" s="3">
-        <v>4986.222222222223</v>
+        <v>1676.388888888889</v>
       </c>
       <c r="C105" s="3">
-        <v>2.416690362683621</v>
+        <v>2.591569538840899</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed report image fmt.; plotting elast. estims.; saving reg. results
</commit_message>
<xml_diff>
--- a/data_analysis/elasticity_results/elasticity.xlsx
+++ b/data_analysis/elasticity_results/elasticity.xlsx
@@ -19,322 +19,322 @@
     <t>Municipality</t>
   </si>
   <si>
-    <t>LatestCensusPop</t>
-  </si>
-  <si>
-    <t>Elasticity</t>
+    <t>MeanPop</t>
+  </si>
+  <si>
+    <t>EstTaxBaseElast</t>
+  </si>
+  <si>
+    <t>Alma</t>
+  </si>
+  <si>
+    <t>Aroostook</t>
+  </si>
+  <si>
+    <t>Atholville</t>
+  </si>
+  <si>
+    <t>Baker-Brook</t>
+  </si>
+  <si>
+    <t>Balmoral</t>
+  </si>
+  <si>
+    <t>Bas-Caraquet</t>
+  </si>
+  <si>
+    <t>Bath</t>
+  </si>
+  <si>
+    <t>Bathurst</t>
+  </si>
+  <si>
+    <t>Belledune</t>
+  </si>
+  <si>
+    <t>Beresford</t>
+  </si>
+  <si>
+    <t>Bertrand</t>
+  </si>
+  <si>
+    <t>Blacks Harbour</t>
+  </si>
+  <si>
+    <t>Blackville</t>
+  </si>
+  <si>
+    <t>Bouctouche</t>
+  </si>
+  <si>
+    <t>Bristol</t>
+  </si>
+  <si>
+    <t>Cambridge-Narrows</t>
+  </si>
+  <si>
+    <t>Campbellton</t>
+  </si>
+  <si>
+    <t>Canterbury</t>
+  </si>
+  <si>
+    <t>Cap-Pelé</t>
+  </si>
+  <si>
+    <t>Caraquet</t>
+  </si>
+  <si>
+    <t>Centreville</t>
+  </si>
+  <si>
+    <t>Charlo</t>
+  </si>
+  <si>
+    <t>Chipman</t>
+  </si>
+  <si>
+    <t>Clair</t>
+  </si>
+  <si>
+    <t>Dalhousie</t>
+  </si>
+  <si>
+    <t>Dieppe</t>
+  </si>
+  <si>
+    <t>Doaktown</t>
+  </si>
+  <si>
+    <t>Dorchester</t>
+  </si>
+  <si>
+    <t>Drummond</t>
+  </si>
+  <si>
+    <t>Edmundston</t>
+  </si>
+  <si>
+    <t>Eel River Crossing</t>
+  </si>
+  <si>
+    <t>Florenceville</t>
+  </si>
+  <si>
+    <t>Florenceville-Bristol</t>
+  </si>
+  <si>
+    <t>Fredericton</t>
+  </si>
+  <si>
+    <t>Fredericton Junction</t>
+  </si>
+  <si>
+    <t>Gagetown</t>
+  </si>
+  <si>
+    <t>Grand Bay-Westfield</t>
+  </si>
+  <si>
+    <t>Grand Falls/Grand-Sault</t>
+  </si>
+  <si>
+    <t>Grand Manan</t>
+  </si>
+  <si>
+    <t>Grande-Anse</t>
+  </si>
+  <si>
+    <t>Hampton</t>
+  </si>
+  <si>
+    <t>Hartland</t>
+  </si>
+  <si>
+    <t>Harvey</t>
+  </si>
+  <si>
+    <t>Hillsborough</t>
+  </si>
+  <si>
+    <t>Kedgwick</t>
+  </si>
+  <si>
+    <t>Lac Baker</t>
+  </si>
+  <si>
+    <t>Lamèque</t>
+  </si>
+  <si>
+    <t>Le Goulet</t>
+  </si>
+  <si>
+    <t>Maisonnette</t>
+  </si>
+  <si>
+    <t>McAdam</t>
+  </si>
+  <si>
+    <t>Meductic</t>
+  </si>
+  <si>
+    <t>Memramcook</t>
+  </si>
+  <si>
+    <t>Millville</t>
+  </si>
+  <si>
+    <t>Minto</t>
+  </si>
+  <si>
+    <t>Miramichi</t>
+  </si>
+  <si>
+    <t>Moncton</t>
+  </si>
+  <si>
+    <t>Nackawic</t>
   </si>
   <si>
     <t>New Maryland</t>
   </si>
   <si>
-    <t>Dorchester</t>
-  </si>
-  <si>
-    <t>Hillsborough</t>
-  </si>
-  <si>
-    <t>Chipman</t>
+    <t>Nigadoo</t>
+  </si>
+  <si>
+    <t>Norton</t>
+  </si>
+  <si>
+    <t>Néguac</t>
+  </si>
+  <si>
+    <t>Oromocto</t>
+  </si>
+  <si>
+    <t>Paquetville</t>
+  </si>
+  <si>
+    <t>Perth-Andover</t>
+  </si>
+  <si>
+    <t>Petit-Rocher</t>
+  </si>
+  <si>
+    <t>Petitcodiac</t>
+  </si>
+  <si>
+    <t>Plaster Rock</t>
+  </si>
+  <si>
+    <t>Pointe-Verte</t>
+  </si>
+  <si>
+    <t>Port Elgin</t>
+  </si>
+  <si>
+    <t>Quispamsis</t>
+  </si>
+  <si>
+    <t>Rexton</t>
+  </si>
+  <si>
+    <t>Richibucto</t>
+  </si>
+  <si>
+    <t>Riverside-Albert</t>
+  </si>
+  <si>
+    <t>Riverview</t>
+  </si>
+  <si>
+    <t>Rivière-Verte</t>
+  </si>
+  <si>
+    <t>Rogersville</t>
+  </si>
+  <si>
+    <t>Rothesay</t>
   </si>
   <si>
     <t>Sackville</t>
   </si>
   <si>
-    <t>Maisonnette</t>
-  </si>
-  <si>
-    <t>Paquetville</t>
-  </si>
-  <si>
-    <t>Belledune</t>
-  </si>
-  <si>
-    <t>Blacks Harbour</t>
+    <t>Saint Andrews</t>
+  </si>
+  <si>
+    <t>Saint George</t>
+  </si>
+  <si>
+    <t>Saint John</t>
+  </si>
+  <si>
+    <t>Saint-André</t>
+  </si>
+  <si>
+    <t>Saint-Antoine</t>
+  </si>
+  <si>
+    <t>Saint-François-de-Madawaska</t>
+  </si>
+  <si>
+    <t>Saint-Hilaire</t>
+  </si>
+  <si>
+    <t>Saint-Isidore</t>
+  </si>
+  <si>
+    <t>Saint-Louis-de-Kent</t>
+  </si>
+  <si>
+    <t>Saint-Léolin</t>
+  </si>
+  <si>
+    <t>Saint-Léonard</t>
+  </si>
+  <si>
+    <t>Saint-Quentin</t>
+  </si>
+  <si>
+    <t>Sainte-Anne-de-Madawaska</t>
+  </si>
+  <si>
+    <t>Sainte-Marie-Saint-Raphaël</t>
+  </si>
+  <si>
+    <t>Salisbury</t>
+  </si>
+  <si>
+    <t>Shediac</t>
   </si>
   <si>
     <t>Shippagan</t>
   </si>
   <si>
-    <t>Richibucto</t>
-  </si>
-  <si>
-    <t>Clair</t>
+    <t>St. Martins</t>
+  </si>
+  <si>
+    <t>St. Stephen</t>
+  </si>
+  <si>
+    <t>Stanley</t>
+  </si>
+  <si>
+    <t>Sussex</t>
   </si>
   <si>
     <t>Sussex Corner</t>
   </si>
   <si>
-    <t>Baker-Brook</t>
-  </si>
-  <si>
-    <t>Gagetown</t>
-  </si>
-  <si>
-    <t>Petit-Rocher</t>
-  </si>
-  <si>
-    <t>Kedgwick</t>
-  </si>
-  <si>
-    <t>Oromocto</t>
-  </si>
-  <si>
-    <t>Bertrand</t>
-  </si>
-  <si>
-    <t>Hartland</t>
-  </si>
-  <si>
-    <t>Saint-Léonard</t>
-  </si>
-  <si>
-    <t>Riverside-Albert</t>
-  </si>
-  <si>
-    <t>Millville</t>
-  </si>
-  <si>
-    <t>Shediac</t>
-  </si>
-  <si>
-    <t>Dieppe</t>
-  </si>
-  <si>
-    <t>Quispamsis</t>
-  </si>
-  <si>
-    <t>Caraquet</t>
+    <t>Tide Head</t>
+  </si>
+  <si>
+    <t>Tracadie-Sheila</t>
+  </si>
+  <si>
+    <t>Tracy</t>
   </si>
   <si>
     <t>Woodstock</t>
-  </si>
-  <si>
-    <t>Cap-Pelé</t>
-  </si>
-  <si>
-    <t>McAdam</t>
-  </si>
-  <si>
-    <t>Cambridge-Narrows</t>
-  </si>
-  <si>
-    <t>Eel River Crossing</t>
-  </si>
-  <si>
-    <t>Grand Falls/Grand-Sault</t>
-  </si>
-  <si>
-    <t>Plaster Rock</t>
-  </si>
-  <si>
-    <t>Moncton</t>
-  </si>
-  <si>
-    <t>St. Martins</t>
-  </si>
-  <si>
-    <t>Port Elgin</t>
-  </si>
-  <si>
-    <t>Blackville</t>
-  </si>
-  <si>
-    <t>Beresford</t>
-  </si>
-  <si>
-    <t>Aroostook</t>
-  </si>
-  <si>
-    <t>Saint-Hilaire</t>
-  </si>
-  <si>
-    <t>Hampton</t>
-  </si>
-  <si>
-    <t>Saint-François-de-Madawaska</t>
-  </si>
-  <si>
-    <t>Miramichi</t>
-  </si>
-  <si>
-    <t>Salisbury</t>
-  </si>
-  <si>
-    <t>Saint George</t>
-  </si>
-  <si>
-    <t>Saint-Isidore</t>
-  </si>
-  <si>
-    <t>Edmundston</t>
-  </si>
-  <si>
-    <t>Perth-Andover</t>
-  </si>
-  <si>
-    <t>Pointe-Verte</t>
-  </si>
-  <si>
-    <t>Lac Baker</t>
-  </si>
-  <si>
-    <t>Bristol</t>
-  </si>
-  <si>
-    <t>Saint-Louis-de-Kent</t>
-  </si>
-  <si>
-    <t>Saint Andrews</t>
-  </si>
-  <si>
-    <t>Minto</t>
-  </si>
-  <si>
-    <t>Riverview</t>
-  </si>
-  <si>
-    <t>Petitcodiac</t>
-  </si>
-  <si>
-    <t>Canterbury</t>
-  </si>
-  <si>
-    <t>Atholville</t>
-  </si>
-  <si>
-    <t>Rothesay</t>
-  </si>
-  <si>
-    <t>Saint-Quentin</t>
-  </si>
-  <si>
-    <t>Sainte-Marie-Saint-Raphaël</t>
-  </si>
-  <si>
-    <t>Florenceville</t>
-  </si>
-  <si>
-    <t>Harvey</t>
-  </si>
-  <si>
-    <t>Centreville</t>
-  </si>
-  <si>
-    <t>Fredericton Junction</t>
-  </si>
-  <si>
-    <t>Tracadie-Sheila</t>
-  </si>
-  <si>
-    <t>Doaktown</t>
-  </si>
-  <si>
-    <t>Sainte-Anne-de-Madawaska</t>
-  </si>
-  <si>
-    <t>Grande-Anse</t>
-  </si>
-  <si>
-    <t>Rivière-Verte</t>
-  </si>
-  <si>
-    <t>Nackawic</t>
-  </si>
-  <si>
-    <t>Charlo</t>
-  </si>
-  <si>
-    <t>Rogersville</t>
-  </si>
-  <si>
-    <t>Drummond</t>
-  </si>
-  <si>
-    <t>Le Goulet</t>
-  </si>
-  <si>
-    <t>Saint-André</t>
-  </si>
-  <si>
-    <t>Campbellton</t>
-  </si>
-  <si>
-    <t>Bath</t>
-  </si>
-  <si>
-    <t>Grand Manan</t>
-  </si>
-  <si>
-    <t>Alma</t>
-  </si>
-  <si>
-    <t>Rexton</t>
-  </si>
-  <si>
-    <t>Grand Bay-Westfield</t>
-  </si>
-  <si>
-    <t>Norton</t>
-  </si>
-  <si>
-    <t>Bouctouche</t>
-  </si>
-  <si>
-    <t>Bathurst</t>
-  </si>
-  <si>
-    <t>Nigadoo</t>
-  </si>
-  <si>
-    <t>St. Stephen</t>
-  </si>
-  <si>
-    <t>Lamèque</t>
-  </si>
-  <si>
-    <t>Saint John</t>
-  </si>
-  <si>
-    <t>Tracy</t>
-  </si>
-  <si>
-    <t>Florenceville-Bristol</t>
-  </si>
-  <si>
-    <t>Saint-Antoine</t>
-  </si>
-  <si>
-    <t>Memramcook</t>
-  </si>
-  <si>
-    <t>Bas-Caraquet</t>
-  </si>
-  <si>
-    <t>Saint-Léolin</t>
-  </si>
-  <si>
-    <t>Stanley</t>
-  </si>
-  <si>
-    <t>Tide Head</t>
-  </si>
-  <si>
-    <t>Fredericton</t>
-  </si>
-  <si>
-    <t>Dalhousie</t>
-  </si>
-  <si>
-    <t>Sussex</t>
-  </si>
-  <si>
-    <t>Balmoral</t>
-  </si>
-  <si>
-    <t>Meductic</t>
-  </si>
-  <si>
-    <t>Néguac</t>
   </si>
 </sst>
 </file>
@@ -409,8 +409,8 @@
   <autoFilter ref="A1:C105"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Municipality" dataDxfId="0"/>
-    <tableColumn id="2" name="LatestCensusPop" dataDxfId="1"/>
-    <tableColumn id="3" name="Elasticity" dataDxfId="1"/>
+    <tableColumn id="2" name="MeanPop" dataDxfId="1"/>
+    <tableColumn id="3" name="EstTaxBaseElast" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -728,10 +728,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="3">
-        <v>4244.111111111111</v>
+        <v>271</v>
       </c>
       <c r="C2" s="3">
-        <v>1.952990849728095</v>
+        <v>1.35725631402635</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -739,10 +739,10 @@
         <v>4</v>
       </c>
       <c r="B3" s="3">
-        <v>1108.333333333333</v>
+        <v>354.6111111111111</v>
       </c>
       <c r="C3" s="3">
-        <v>4.37942380018478</v>
+        <v>6.887094143371944</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -750,10 +750,10 @@
         <v>5</v>
       </c>
       <c r="B4" s="3">
-        <v>1298.388888888889</v>
+        <v>1695.222222222222</v>
       </c>
       <c r="C4" s="3">
-        <v>3.176899455564953</v>
+        <v>0.9621589682907417</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -761,10 +761,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="3">
-        <v>1308.944444444444</v>
+        <v>575.1176470588235</v>
       </c>
       <c r="C5" s="3">
-        <v>2.978555887229455</v>
+        <v>3.945005804783354</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -772,10 +772,10 @@
         <v>7</v>
       </c>
       <c r="B6" s="3">
-        <v>5419</v>
+        <v>1770.055555555556</v>
       </c>
       <c r="C6" s="3">
-        <v>1.173257410267234</v>
+        <v>3.998255047180202</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -783,10 +783,10 @@
         <v>8</v>
       </c>
       <c r="B7" s="3">
-        <v>589.5555555555555</v>
+        <v>1510.111111111111</v>
       </c>
       <c r="C7" s="3">
-        <v>4.246522363577463</v>
+        <v>4.546150634098066</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -794,10 +794,10 @@
         <v>9</v>
       </c>
       <c r="B8" s="3">
-        <v>688.2222222222222</v>
+        <v>543.2777777777778</v>
       </c>
       <c r="C8" s="3">
-        <v>2.704154469791415</v>
+        <v>3.8898703995655</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -805,10 +805,10 @@
         <v>10</v>
       </c>
       <c r="B9" s="3">
-        <v>1719.277777777778</v>
+        <v>12698.77777777778</v>
       </c>
       <c r="C9" s="3">
-        <v>-0.03230382618528604</v>
+        <v>1.783866583660905</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -816,10 +816,10 @@
         <v>11</v>
       </c>
       <c r="B10" s="3">
-        <v>1003.333333333333</v>
+        <v>1719.277777777778</v>
       </c>
       <c r="C10" s="3">
-        <v>2.327125813468714</v>
+        <v>-0.03230382618528604</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -827,10 +827,10 @@
         <v>12</v>
       </c>
       <c r="B11" s="3">
-        <v>2741.777777777778</v>
+        <v>4388.333333333333</v>
       </c>
       <c r="C11" s="3">
-        <v>1.826592004438217</v>
+        <v>3.154566206059836</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -838,10 +838,10 @@
         <v>13</v>
       </c>
       <c r="B12" s="3">
-        <v>1314.277777777778</v>
+        <v>1215.833333333333</v>
       </c>
       <c r="C12" s="3">
-        <v>1.865748618876328</v>
+        <v>4.520087914571928</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -849,10 +849,10 @@
         <v>14</v>
       </c>
       <c r="B13" s="3">
-        <v>854.9411764705883</v>
+        <v>1003.333333333333</v>
       </c>
       <c r="C13" s="3">
-        <v>2.194402962374678</v>
+        <v>2.327125813468714</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -860,10 +860,10 @@
         <v>15</v>
       </c>
       <c r="B14" s="3">
-        <v>1411.222222222222</v>
+        <v>966.9444444444445</v>
       </c>
       <c r="C14" s="3">
-        <v>2.741347663741911</v>
+        <v>3.633383811351338</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -871,10 +871,10 @@
         <v>16</v>
       </c>
       <c r="B15" s="3">
-        <v>575.1176470588235</v>
+        <v>2408.055555555556</v>
       </c>
       <c r="C15" s="3">
-        <v>3.945005804783354</v>
+        <v>1.940028840493857</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -882,10 +882,10 @@
         <v>17</v>
       </c>
       <c r="B16" s="3">
-        <v>697</v>
+        <v>704.5</v>
       </c>
       <c r="C16" s="3">
-        <v>1.94581028903611</v>
+        <v>2.838654908492098</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -893,10 +893,10 @@
         <v>18</v>
       </c>
       <c r="B17" s="3">
-        <v>1955.555555555556</v>
+        <v>645.2777777777778</v>
       </c>
       <c r="C17" s="3">
-        <v>3.707019874209061</v>
+        <v>0.8796179759578735</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -904,10 +904,10 @@
         <v>19</v>
       </c>
       <c r="B18" s="3">
-        <v>1161.5</v>
+        <v>7539.722222222223</v>
       </c>
       <c r="C18" s="3">
-        <v>4.910995710330457</v>
+        <v>2.369143003552924</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -915,10 +915,10 @@
         <v>20</v>
       </c>
       <c r="B19" s="3">
-        <v>8862.111111111111</v>
+        <v>366.0555555555555</v>
       </c>
       <c r="C19" s="3">
-        <v>1.015540391140557</v>
+        <v>5.145604421258335</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -926,10 +926,10 @@
         <v>21</v>
       </c>
       <c r="B20" s="3">
-        <v>1215.833333333333</v>
+        <v>2289.888888888889</v>
       </c>
       <c r="C20" s="3">
-        <v>4.520087914571928</v>
+        <v>2.114770802958085</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -937,10 +937,10 @@
         <v>22</v>
       </c>
       <c r="B21" s="3">
-        <v>932</v>
+        <v>4304.722222222223</v>
       </c>
       <c r="C21" s="3">
-        <v>1.756911632289728</v>
+        <v>2.060478459612275</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -948,10 +948,10 @@
         <v>23</v>
       </c>
       <c r="B22" s="3">
-        <v>1363.166666666667</v>
+        <v>540.8888888888889</v>
       </c>
       <c r="C22" s="3">
-        <v>3.418821882174067</v>
+        <v>2.262430506182488</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -959,10 +959,10 @@
         <v>24</v>
       </c>
       <c r="B23" s="3">
-        <v>360.3333333333333</v>
+        <v>1404.611111111111</v>
       </c>
       <c r="C23" s="3">
-        <v>3.257262687746987</v>
+        <v>3.339439589950414</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -970,10 +970,10 @@
         <v>25</v>
       </c>
       <c r="B24" s="3">
-        <v>304.5555555555555</v>
+        <v>1308.944444444444</v>
       </c>
       <c r="C24" s="3">
-        <v>5.423905213307876</v>
+        <v>2.978555887229455</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -981,10 +981,10 @@
         <v>26</v>
       </c>
       <c r="B25" s="3">
-        <v>5576.888888888889</v>
+        <v>854.9411764705883</v>
       </c>
       <c r="C25" s="3">
-        <v>1.586326401123529</v>
+        <v>2.194402962374678</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -992,10 +992,10 @@
         <v>27</v>
       </c>
       <c r="B26" s="3">
-        <v>19142.27777777778</v>
+        <v>3735.055555555556</v>
       </c>
       <c r="C26" s="3">
-        <v>0.9990234685779513</v>
+        <v>1.624458607049494</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1003,10 +1003,10 @@
         <v>28</v>
       </c>
       <c r="B27" s="3">
-        <v>15794.88888888889</v>
+        <v>19142.27777777778</v>
       </c>
       <c r="C27" s="3">
-        <v>1.732085870349754</v>
+        <v>0.9990234685779513</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1014,10 +1014,10 @@
         <v>29</v>
       </c>
       <c r="B28" s="3">
-        <v>4304.722222222223</v>
+        <v>878.3888888888889</v>
       </c>
       <c r="C28" s="3">
-        <v>2.060478459612275</v>
+        <v>2.269547133639938</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -1025,10 +1025,10 @@
         <v>30</v>
       </c>
       <c r="B29" s="3">
-        <v>5174.166666666667</v>
+        <v>1108.333333333333</v>
       </c>
       <c r="C29" s="3">
-        <v>1.701667528830308</v>
+        <v>4.37942380018478</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1036,10 +1036,10 @@
         <v>31</v>
       </c>
       <c r="B30" s="3">
-        <v>2289.888888888889</v>
+        <v>847.2777777777778</v>
       </c>
       <c r="C30" s="3">
-        <v>2.114770802958085</v>
+        <v>2.572031666180989</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1047,10 +1047,10 @@
         <v>32</v>
       </c>
       <c r="B31" s="3">
-        <v>1381</v>
+        <v>16813.55555555555</v>
       </c>
       <c r="C31" s="3">
-        <v>5.41825371553831</v>
+        <v>1.824416770379819</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1058,10 +1058,10 @@
         <v>33</v>
       </c>
       <c r="B32" s="3">
-        <v>645.2777777777778</v>
+        <v>1382.111111111111</v>
       </c>
       <c r="C32" s="3">
-        <v>0.8796179759578735</v>
+        <v>4.898482965635322</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1069,10 +1069,10 @@
         <v>34</v>
       </c>
       <c r="B33" s="3">
-        <v>1382.111111111111</v>
+        <v>765.875</v>
       </c>
       <c r="C33" s="3">
-        <v>4.898482965635322</v>
+        <v>0.5731196185501</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1080,10 +1080,10 @@
         <v>35</v>
       </c>
       <c r="B34" s="3">
-        <v>5723.611111111111</v>
+        <v>1598.5</v>
       </c>
       <c r="C34" s="3">
-        <v>1.509234673336074</v>
+        <v>0.5343369108736038</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1091,10 +1091,10 @@
         <v>36</v>
       </c>
       <c r="B35" s="3">
-        <v>1148.666666666667</v>
+        <v>52043.83333333334</v>
       </c>
       <c r="C35" s="3">
-        <v>2.96719973826789</v>
+        <v>0.9589643109472232</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1102,10 +1102,10 @@
         <v>37</v>
       </c>
       <c r="B36" s="3">
-        <v>65204.44444444445</v>
+        <v>721.0555555555555</v>
       </c>
       <c r="C36" s="3">
-        <v>1.277468593367812</v>
+        <v>3.327938956505582</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1113,10 +1113,10 @@
         <v>38</v>
       </c>
       <c r="B37" s="3">
-        <v>349.6666666666667</v>
+        <v>697</v>
       </c>
       <c r="C37" s="3">
-        <v>2.678940404510244</v>
+        <v>1.94581028903611</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1124,10 +1124,10 @@
         <v>39</v>
       </c>
       <c r="B38" s="3">
-        <v>433</v>
+        <v>4986.222222222223</v>
       </c>
       <c r="C38" s="3">
-        <v>3.283537035349036</v>
+        <v>2.416673700971703</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1135,10 +1135,10 @@
         <v>40</v>
       </c>
       <c r="B39" s="3">
-        <v>966.9444444444445</v>
+        <v>5723.611111111111</v>
       </c>
       <c r="C39" s="3">
-        <v>3.633383811351338</v>
+        <v>1.509234673336074</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1146,10 +1146,10 @@
         <v>41</v>
       </c>
       <c r="B40" s="3">
-        <v>4388.333333333333</v>
+        <v>2469.388888888889</v>
       </c>
       <c r="C40" s="3">
-        <v>3.154566206059836</v>
+        <v>2.131539285800402</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1157,10 +1157,10 @@
         <v>42</v>
       </c>
       <c r="B41" s="3">
-        <v>354.6111111111111</v>
+        <v>827.3888888888889</v>
       </c>
       <c r="C41" s="3">
-        <v>6.887094143371944</v>
+        <v>3.933745317083301</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1168,10 +1168,10 @@
         <v>43</v>
       </c>
       <c r="B42" s="3">
-        <v>246.4117647058823</v>
+        <v>4127.166666666667</v>
       </c>
       <c r="C42" s="3">
-        <v>1.158124226992246</v>
+        <v>2.115583174554904</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1179,10 +1179,10 @@
         <v>44</v>
       </c>
       <c r="B43" s="3">
-        <v>4127.166666666667</v>
+        <v>932</v>
       </c>
       <c r="C43" s="3">
-        <v>2.115583174554904</v>
+        <v>1.756911632289728</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1190,10 +1190,10 @@
         <v>45</v>
       </c>
       <c r="B44" s="3">
-        <v>565.0588235294117</v>
+        <v>360.1111111111111</v>
       </c>
       <c r="C44" s="3">
-        <v>2.264175256123465</v>
+        <v>3.39133184220729</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1201,10 +1201,10 @@
         <v>46</v>
       </c>
       <c r="B45" s="3">
-        <v>18208.16666666667</v>
+        <v>1298.388888888889</v>
       </c>
       <c r="C45" s="3">
-        <v>1.784736035585024</v>
+        <v>3.176899455564953</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1212,10 +1212,10 @@
         <v>47</v>
       </c>
       <c r="B46" s="3">
-        <v>2075.555555555556</v>
+        <v>1161.5</v>
       </c>
       <c r="C46" s="3">
-        <v>2.260271692479443</v>
+        <v>4.910995710330457</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1223,10 +1223,10 @@
         <v>48</v>
       </c>
       <c r="B47" s="3">
-        <v>1480.333333333333</v>
+        <v>489.0555555555555</v>
       </c>
       <c r="C47" s="3">
-        <v>1.692927509218713</v>
+        <v>3.008838168732169</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1234,10 +1234,10 @@
         <v>49</v>
       </c>
       <c r="B48" s="3">
-        <v>812.8333333333334</v>
+        <v>1469.222222222222</v>
       </c>
       <c r="C48" s="3">
-        <v>3.336739651606498</v>
+        <v>2.720345156539985</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1245,10 +1245,10 @@
         <v>50</v>
       </c>
       <c r="B49" s="3">
-        <v>16813.55555555555</v>
+        <v>898.9444444444445</v>
       </c>
       <c r="C49" s="3">
-        <v>1.824416770379819</v>
+        <v>8.023132541218956</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1256,10 +1256,10 @@
         <v>51</v>
       </c>
       <c r="B50" s="3">
-        <v>1787.444444444444</v>
+        <v>589.5555555555555</v>
       </c>
       <c r="C50" s="3">
-        <v>2.554172184965163</v>
+        <v>4.246522363577463</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1267,10 +1267,10 @@
         <v>52</v>
       </c>
       <c r="B51" s="3">
-        <v>994.7777777777778</v>
+        <v>1381</v>
       </c>
       <c r="C51" s="3">
-        <v>5.274725717453601</v>
+        <v>5.41825371553831</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1278,10 +1278,10 @@
         <v>53</v>
       </c>
       <c r="B52" s="3">
-        <v>489.0555555555555</v>
+        <v>198.0555555555555</v>
       </c>
       <c r="C52" s="3">
-        <v>3.008838168732169</v>
+        <v>2.114741053280721</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1289,10 +1289,10 @@
         <v>54</v>
       </c>
       <c r="B53" s="3">
-        <v>704.5</v>
+        <v>4762.055555555556</v>
       </c>
       <c r="C53" s="3">
-        <v>2.838654908492098</v>
+        <v>3.281235553054098</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1300,10 +1300,10 @@
         <v>55</v>
       </c>
       <c r="B54" s="3">
-        <v>950.3333333333334</v>
+        <v>304.5555555555555</v>
       </c>
       <c r="C54" s="3">
-        <v>2.968406732834274</v>
+        <v>5.423905213307876</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1311,10 +1311,10 @@
         <v>56</v>
       </c>
       <c r="B55" s="3">
-        <v>1820.388888888889</v>
+        <v>2657.555555555556</v>
       </c>
       <c r="C55" s="3">
-        <v>0.571311153813002</v>
+        <v>4.197561285620755</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1322,10 +1322,10 @@
         <v>57</v>
       </c>
       <c r="B56" s="3">
-        <v>2657.555555555556</v>
+        <v>18208.16666666667</v>
       </c>
       <c r="C56" s="3">
-        <v>4.197561285620755</v>
+        <v>1.784736035585024</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1333,10 +1333,10 @@
         <v>58</v>
       </c>
       <c r="B57" s="3">
-        <v>18092.33333333333</v>
+        <v>65204.44444444445</v>
       </c>
       <c r="C57" s="3">
-        <v>2.276943870757617</v>
+        <v>1.277468593367812</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1344,10 +1344,10 @@
         <v>59</v>
       </c>
       <c r="B58" s="3">
-        <v>1406.222222222222</v>
+        <v>1029.5</v>
       </c>
       <c r="C58" s="3">
-        <v>2.606731384182654</v>
+        <v>0.9283714397010021</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1355,10 +1355,10 @@
         <v>60</v>
       </c>
       <c r="B59" s="3">
-        <v>366.0555555555555</v>
+        <v>4244.111111111111</v>
       </c>
       <c r="C59" s="3">
-        <v>5.145604421258335</v>
+        <v>1.952990849728095</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1366,10 +1366,10 @@
         <v>61</v>
       </c>
       <c r="B60" s="3">
-        <v>1695.222222222222</v>
+        <v>953.5555555555555</v>
       </c>
       <c r="C60" s="3">
-        <v>0.9621589682907417</v>
+        <v>4.038286161672137</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1377,10 +1377,10 @@
         <v>62</v>
       </c>
       <c r="B61" s="3">
-        <v>11635.55555555555</v>
+        <v>1344.444444444444</v>
       </c>
       <c r="C61" s="3">
-        <v>1.409696492634694</v>
+        <v>3.921826183576595</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1388,10 +1388,10 @@
         <v>63</v>
       </c>
       <c r="B62" s="3">
-        <v>2240.222222222222</v>
+        <v>1676.388888888889</v>
       </c>
       <c r="C62" s="3">
-        <v>3.08706349343197</v>
+        <v>2.591569538840899</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1399,10 +1399,10 @@
         <v>64</v>
       </c>
       <c r="B63" s="3">
-        <v>1021.222222222222</v>
+        <v>8862.111111111111</v>
       </c>
       <c r="C63" s="3">
-        <v>6.007627490035411</v>
+        <v>1.015540391140557</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1410,10 +1410,10 @@
         <v>65</v>
       </c>
       <c r="B64" s="3">
-        <v>765.875</v>
+        <v>688.2222222222222</v>
       </c>
       <c r="C64" s="3">
-        <v>0.5731196185501</v>
+        <v>2.704154469791415</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1421,10 +1421,10 @@
         <v>66</v>
       </c>
       <c r="B65" s="3">
-        <v>360.1111111111111</v>
+        <v>1787.444444444444</v>
       </c>
       <c r="C65" s="3">
-        <v>3.39133184220729</v>
+        <v>2.554172184965163</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1432,10 +1432,10 @@
         <v>67</v>
       </c>
       <c r="B66" s="3">
-        <v>540.8888888888889</v>
+        <v>1955.555555555556</v>
       </c>
       <c r="C66" s="3">
-        <v>2.262430506182488</v>
+        <v>3.707019874209061</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1443,10 +1443,10 @@
         <v>68</v>
       </c>
       <c r="B67" s="3">
-        <v>721.0555555555555</v>
+        <v>1406.222222222222</v>
       </c>
       <c r="C67" s="3">
-        <v>3.327938956505582</v>
+        <v>2.606731384182654</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1454,10 +1454,10 @@
         <v>69</v>
       </c>
       <c r="B68" s="3">
-        <v>4690</v>
+        <v>1148.666666666667</v>
       </c>
       <c r="C68" s="3">
-        <v>1.939948131515448</v>
+        <v>2.96719973826789</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1465,10 +1465,10 @@
         <v>70</v>
       </c>
       <c r="B69" s="3">
-        <v>878.3888888888889</v>
+        <v>994.7777777777778</v>
       </c>
       <c r="C69" s="3">
-        <v>2.269547133639938</v>
+        <v>5.274725717453601</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1476,10 +1476,10 @@
         <v>71</v>
       </c>
       <c r="B70" s="3">
-        <v>1087.055555555556</v>
+        <v>433</v>
       </c>
       <c r="C70" s="3">
-        <v>4.759575287918111</v>
+        <v>3.283537035349036</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1487,10 +1487,10 @@
         <v>72</v>
       </c>
       <c r="B71" s="3">
-        <v>827.3888888888889</v>
+        <v>15794.88888888889</v>
       </c>
       <c r="C71" s="3">
-        <v>3.933745317083301</v>
+        <v>1.732085870349754</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -1498,10 +1498,10 @@
         <v>73</v>
       </c>
       <c r="B72" s="3">
-        <v>805.1666666666666</v>
+        <v>845.8888888888889</v>
       </c>
       <c r="C72" s="3">
-        <v>3.882179446133341</v>
+        <v>1.809890164114266</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -1509,10 +1509,10 @@
         <v>74</v>
       </c>
       <c r="B73" s="3">
-        <v>1029.5</v>
+        <v>1314.277777777778</v>
       </c>
       <c r="C73" s="3">
-        <v>0.9283714397010021</v>
+        <v>1.865748618876328</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -1520,10 +1520,10 @@
         <v>75</v>
       </c>
       <c r="B74" s="3">
-        <v>1404.611111111111</v>
+        <v>360.3333333333333</v>
       </c>
       <c r="C74" s="3">
-        <v>3.339439589950414</v>
+        <v>3.257262687746987</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -1531,10 +1531,10 @@
         <v>76</v>
       </c>
       <c r="B75" s="3">
-        <v>1208.611111111111</v>
+        <v>18092.33333333333</v>
       </c>
       <c r="C75" s="3">
-        <v>4.085181848712212</v>
+        <v>2.276943870757617</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -1542,10 +1542,10 @@
         <v>77</v>
       </c>
       <c r="B76" s="3">
-        <v>847.2777777777778</v>
+        <v>805.1666666666666</v>
       </c>
       <c r="C76" s="3">
-        <v>2.572031666180989</v>
+        <v>3.882179446133341</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -1553,10 +1553,10 @@
         <v>78</v>
       </c>
       <c r="B77" s="3">
-        <v>898.9444444444445</v>
+        <v>1208.611111111111</v>
       </c>
       <c r="C77" s="3">
-        <v>8.023132541218956</v>
+        <v>4.085181848712212</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -1564,10 +1564,10 @@
         <v>79</v>
       </c>
       <c r="B78" s="3">
-        <v>426.5</v>
+        <v>11635.55555555555</v>
       </c>
       <c r="C78" s="3">
-        <v>4.635793554937599</v>
+        <v>1.409696492634694</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -1575,10 +1575,10 @@
         <v>80</v>
       </c>
       <c r="B79" s="3">
-        <v>7539.722222222223</v>
+        <v>5419</v>
       </c>
       <c r="C79" s="3">
-        <v>2.369143003552924</v>
+        <v>1.173257410267234</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -1586,10 +1586,10 @@
         <v>81</v>
       </c>
       <c r="B80" s="3">
-        <v>543.2777777777778</v>
+        <v>1820.388888888889</v>
       </c>
       <c r="C80" s="3">
-        <v>3.8898703995655</v>
+        <v>0.571311153813002</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -1597,10 +1597,10 @@
         <v>82</v>
       </c>
       <c r="B81" s="3">
-        <v>2469.388888888889</v>
+        <v>1480.333333333333</v>
       </c>
       <c r="C81" s="3">
-        <v>2.131539285800402</v>
+        <v>1.692927509218713</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -1608,10 +1608,10 @@
         <v>83</v>
       </c>
       <c r="B82" s="3">
-        <v>271</v>
+        <v>69425.38888888889</v>
       </c>
       <c r="C82" s="3">
-        <v>1.35725631402635</v>
+        <v>1.473476127805057</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -1619,10 +1619,10 @@
         <v>84</v>
       </c>
       <c r="B83" s="3">
-        <v>845.8888888888889</v>
+        <v>426.5</v>
       </c>
       <c r="C83" s="3">
-        <v>1.809890164114266</v>
+        <v>4.635793554937599</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -1630,10 +1630,10 @@
         <v>85</v>
       </c>
       <c r="B84" s="3">
-        <v>4986.222222222223</v>
+        <v>1599.111111111111</v>
       </c>
       <c r="C84" s="3">
-        <v>2.416673700971703</v>
+        <v>2.981145719466401</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -1641,10 +1641,10 @@
         <v>86</v>
       </c>
       <c r="B85" s="3">
-        <v>1344.444444444444</v>
+        <v>565.0588235294117</v>
       </c>
       <c r="C85" s="3">
-        <v>3.921826183576595</v>
+        <v>2.264175256123465</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -1652,10 +1652,10 @@
         <v>87</v>
       </c>
       <c r="B86" s="3">
-        <v>2408.055555555556</v>
+        <v>246.4117647058823</v>
       </c>
       <c r="C86" s="3">
-        <v>1.940028840493857</v>
+        <v>1.158124226992246</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -1663,10 +1663,10 @@
         <v>88</v>
       </c>
       <c r="B87" s="3">
-        <v>12698.77777777778</v>
+        <v>812.8333333333334</v>
       </c>
       <c r="C87" s="3">
-        <v>1.783866583660905</v>
+        <v>3.336739651606498</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -1674,10 +1674,10 @@
         <v>89</v>
       </c>
       <c r="B88" s="3">
-        <v>953.5555555555555</v>
+        <v>950.3333333333334</v>
       </c>
       <c r="C88" s="3">
-        <v>4.038286161672137</v>
+        <v>2.968406732834274</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -1685,10 +1685,10 @@
         <v>90</v>
       </c>
       <c r="B89" s="3">
-        <v>4738.722222222223</v>
+        <v>718.3333333333334</v>
       </c>
       <c r="C89" s="3">
-        <v>2.020898137479048</v>
+        <v>7.020103735428291</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -1696,10 +1696,10 @@
         <v>91</v>
       </c>
       <c r="B90" s="3">
-        <v>1469.222222222222</v>
+        <v>1363.166666666667</v>
       </c>
       <c r="C90" s="3">
-        <v>2.720345156539985</v>
+        <v>3.418821882174067</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -1707,10 +1707,10 @@
         <v>92</v>
       </c>
       <c r="B91" s="3">
-        <v>69425.38888888889</v>
+        <v>2240.222222222222</v>
       </c>
       <c r="C91" s="3">
-        <v>1.473476127805057</v>
+        <v>3.08706349343197</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -1718,10 +1718,10 @@
         <v>93</v>
       </c>
       <c r="B92" s="3">
-        <v>610.0555555555555</v>
+        <v>1087.055555555556</v>
       </c>
       <c r="C92" s="3">
-        <v>4.675489641386824</v>
+        <v>4.759575287918111</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -1729,10 +1729,10 @@
         <v>94</v>
       </c>
       <c r="B93" s="3">
-        <v>1598.5</v>
+        <v>1021.222222222222</v>
       </c>
       <c r="C93" s="3">
-        <v>0.5343369108736038</v>
+        <v>6.007627490035411</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -1740,10 +1740,10 @@
         <v>95</v>
       </c>
       <c r="B94" s="3">
-        <v>1599.111111111111</v>
+        <v>2075.555555555556</v>
       </c>
       <c r="C94" s="3">
-        <v>2.981145719466401</v>
+        <v>2.260271692479443</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -1751,10 +1751,10 @@
         <v>96</v>
       </c>
       <c r="B95" s="3">
-        <v>4762.055555555556</v>
+        <v>5576.888888888889</v>
       </c>
       <c r="C95" s="3">
-        <v>3.281235553054098</v>
+        <v>1.586326401123529</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -1762,10 +1762,10 @@
         <v>97</v>
       </c>
       <c r="B96" s="3">
-        <v>1510.111111111111</v>
+        <v>2741.777777777778</v>
       </c>
       <c r="C96" s="3">
-        <v>4.546150634098066</v>
+        <v>1.826592004438217</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -1773,10 +1773,10 @@
         <v>98</v>
       </c>
       <c r="B97" s="3">
-        <v>718.3333333333334</v>
+        <v>349.6666666666667</v>
       </c>
       <c r="C97" s="3">
-        <v>7.020103735428291</v>
+        <v>2.678940404510244</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -1784,10 +1784,10 @@
         <v>99</v>
       </c>
       <c r="B98" s="3">
-        <v>429.7222222222222</v>
+        <v>4738.722222222223</v>
       </c>
       <c r="C98" s="3">
-        <v>2.454632666991825</v>
+        <v>2.020898137479048</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -1795,10 +1795,10 @@
         <v>100</v>
       </c>
       <c r="B99" s="3">
-        <v>1071.666666666667</v>
+        <v>429.7222222222222</v>
       </c>
       <c r="C99" s="3">
-        <v>3.382878491978183</v>
+        <v>2.454632666991825</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -1806,10 +1806,10 @@
         <v>101</v>
       </c>
       <c r="B100" s="3">
-        <v>52043.83333333334</v>
+        <v>4262.444444444444</v>
       </c>
       <c r="C100" s="3">
-        <v>0.9589643109472232</v>
+        <v>1.518729168682847</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -1817,10 +1817,10 @@
         <v>102</v>
       </c>
       <c r="B101" s="3">
-        <v>3735.055555555556</v>
+        <v>1411.222222222222</v>
       </c>
       <c r="C101" s="3">
-        <v>1.624458607049494</v>
+        <v>2.741347663741911</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -1828,10 +1828,10 @@
         <v>103</v>
       </c>
       <c r="B102" s="3">
-        <v>4262.444444444444</v>
+        <v>1071.666666666667</v>
       </c>
       <c r="C102" s="3">
-        <v>1.518729168682847</v>
+        <v>3.382878491978183</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -1839,10 +1839,10 @@
         <v>104</v>
       </c>
       <c r="B103" s="3">
-        <v>1770.055555555556</v>
+        <v>4690</v>
       </c>
       <c r="C103" s="3">
-        <v>3.998255047180202</v>
+        <v>1.939948131515448</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -1850,10 +1850,10 @@
         <v>105</v>
       </c>
       <c r="B104" s="3">
-        <v>198.0555555555555</v>
+        <v>610.0555555555555</v>
       </c>
       <c r="C104" s="3">
-        <v>2.114741053280721</v>
+        <v>4.675489641386824</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -1861,10 +1861,10 @@
         <v>106</v>
       </c>
       <c r="B105" s="3">
-        <v>1676.388888888889</v>
+        <v>5174.166666666667</v>
       </c>
       <c r="C105" s="3">
-        <v>2.591569538840899</v>
+        <v>1.701667528830308</v>
       </c>
     </row>
   </sheetData>

</xml_diff>